<commit_message>
Update module 5 template
</commit_message>
<xml_diff>
--- a/public/templates/NHWA_Module_5.xlsx
+++ b/public/templates/NHWA_Module_5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\NHWA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\NHWA\Originals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568ED9E5-4E0F-4374-A05A-BC597CA8D6E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45940A1B-BC03-446D-8609-640A55972FB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="D8NLvK0a2zIADanhZ9TwvH5vsYkmadwkU44pHflONSE2WP8HiyNEmpWYSjEZss1+UZ+xu9L5Oen+ioj0nOts3g==" workbookSaltValue="X5E0+xThdEGqXq8WVwCqrQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="836">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2810,6 +2810,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -2838,7 +2839,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -3265,7 +3265,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB266"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -3280,11 +3280,12 @@
     <col min="8" max="9" width="12.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="24.5703125" style="4" customWidth="1"/>
     <col min="11" max="12" width="14.28515625" style="4" customWidth="1"/>
-    <col min="13" max="17" width="9.140625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="12" style="4" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" style="4" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="12" style="4" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="12.140625" style="4" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="9.7109375" style="4" hidden="1" customWidth="1"/>
     <col min="24" max="35" width="9.140625" style="4" hidden="1" customWidth="1"/>
@@ -3293,25 +3294,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="29" t="s">
         <v>835</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -3338,22 +3339,22 @@
       </c>
     </row>
     <row r="2" spans="1:33" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>764</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -3531,11 +3532,11 @@
     <row r="6" spans="1:33" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
       <c r="AA6" s="4" t="s">
         <v>109</v>
       </c>
@@ -3562,33 +3563,33 @@
       </c>
     </row>
     <row r="7" spans="1:33" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="32" t="s">
         <v>750</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="34" t="s">
         <v>751</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="36" t="s">
         <v>752</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="33" t="s">
+      <c r="F7" s="37"/>
+      <c r="G7" s="34" t="s">
         <v>753</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="36" t="s">
         <v>754</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="33" t="s">
+      <c r="I7" s="37"/>
+      <c r="J7" s="34" t="s">
         <v>755</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="36" t="s">
         <v>756</v>
       </c>
-      <c r="L7" s="36"/>
+      <c r="L7" s="37"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="16"/>
@@ -3622,23 +3623,23 @@
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="34"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="34"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="19" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="34"/>
+      <c r="J8" s="35"/>
       <c r="K8" s="21" t="s">
         <v>10</v>
       </c>
@@ -10613,7 +10614,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="inLRJbx2w4Oa9EXnraj0Dq5FGu0MUX/U1VEMfUtYy7mg/Hzs+TVb/2OI5jh1C6AGYxYweQGBgbPCmFtamgVdVg==" saltValue="E6NVbNrsqpHX1RyyU98L7Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="I59ROVBstQo5MFLl7seOlwH97/8trwXUUwg/j8hrzmDt4hwT+gWPi2GFb6pjGOZjwM+bFz7qyb4hSAVWakYqIw==" saltValue="i+4wjmCbRDAe0olRhH+r5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="12">
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:O2"/>
@@ -10697,38 +10698,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>764</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="12" t="e">
         <f>'Entry into Labour Market'!X2</f>
         <v>#N/A</v>
@@ -10784,57 +10785,57 @@
       <c r="O6" s="12"/>
     </row>
     <row r="7" spans="2:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="38" t="s">
         <v>750</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="34" t="s">
         <v>762</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="36" t="s">
         <v>762</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="33" t="s">
+      <c r="F7" s="37"/>
+      <c r="G7" s="34" t="s">
         <v>757</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="34" t="s">
         <v>758</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="36" t="s">
         <v>758</v>
       </c>
-      <c r="J7" s="36"/>
-      <c r="K7" s="33" t="s">
+      <c r="J7" s="37"/>
+      <c r="K7" s="34" t="s">
         <v>763</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="L7" s="36" t="s">
         <v>763</v>
       </c>
-      <c r="M7" s="36"/>
+      <c r="M7" s="37"/>
       <c r="O7" s="12"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="34"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="23" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="34"/>
+      <c r="K8" s="35"/>
       <c r="L8" s="23" t="s">
         <v>10</v>
       </c>

</xml_diff>